<commit_message>
Inserted data and modified erd
</commit_message>
<xml_diff>
--- a/documents/normalizeddata.xlsx
+++ b/documents/normalizeddata.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\420-240-DW (Infra II)\project normalized data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b4b11a24c2163ac/Desktop/Computer science/sql2/finalProject/fall2023database2finalproject/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{03AC75C9-ECA2-4179-9FB2-F39E0F766300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="14_{03AC75C9-ECA2-4179-9FB2-F39E0F766300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB199002-183A-428B-9E09-C13B2F708552}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F772C2C-AA53-E44B-82EB-3E383105B2CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F772C2C-AA53-E44B-82EB-3E383105B2CA}"/>
   </bookViews>
   <sheets>
     <sheet name="order info" sheetId="2" r:id="rId1"/>
     <sheet name="Inventory info" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -897,28 +896,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5EF3CE-9498-419C-B302-D50D5D741EA5}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="19.375" customWidth="1"/>
-    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="1" max="1" width="19.59765625" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" customWidth="1"/>
+    <col min="3" max="3" width="28.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.8984375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="11" max="11" width="12.875" customWidth="1"/>
-    <col min="12" max="12" width="19.375" customWidth="1"/>
+    <col min="9" max="9" width="10.3984375" customWidth="1"/>
+    <col min="11" max="11" width="12.8984375" customWidth="1"/>
+    <col min="12" max="12" width="19.3984375" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
+    <col min="14" max="14" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1040,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1120,7 +1119,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1158,7 +1157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1240,7 +1239,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1281,7 +1280,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1310,7 +1309,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1342,7 +1341,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1412,7 +1411,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1488,7 +1487,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1681,7 +1680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -1716,7 +1715,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>145</v>
       </c>
@@ -1839,7 +1838,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>146</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>124</v>
       </c>
@@ -1882,7 +1881,7 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>127</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>137</v>
       </c>
@@ -1938,7 +1937,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>138</v>
       </c>
@@ -1995,22 +1994,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38707693-70B7-4E89-8DFC-87C356C7D744}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.09765625" customWidth="1"/>
     <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
-    <col min="6" max="6" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" customWidth="1"/>
+    <col min="6" max="6" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2080,7 +2079,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2108,7 +2107,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -2136,7 +2135,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>118</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -2178,7 +2177,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -2220,7 +2219,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -2234,7 +2233,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -2248,7 +2247,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>118</v>
       </c>

</xml_diff>